<commit_message>
cleanup and update docs
</commit_message>
<xml_diff>
--- a/vignettes/articles/report_norm.xlsx
+++ b/vignettes/articles/report_norm.xlsx
@@ -616,7 +616,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="18.711"/>
-    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="26.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="27.711"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -639,7 +639,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-30 17:04:40.73049</t>
+          <t>2025-06-16 10:45:05.079195</t>
         </is>
       </c>
     </row>

</xml_diff>